<commit_message>
finalize files for upload
</commit_message>
<xml_diff>
--- a/data-raw/metadata/survey_locations_metadata.xlsx
+++ b/data-raw/metadata/survey_locations_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/feather-mini-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665D2350-C66E-B04E-B333-784F6592894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346C9639-4D15-6D40-AA80-0345B15B0DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61180" yWindow="1660" windowWidth="32240" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29660" yWindow="500" windowWidth="32240" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -352,10 +352,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -558,7 +554,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -877,13 +873,13 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>50</v>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>38</v>
@@ -894,8 +890,8 @@
       <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>44</v>
+      <c r="G8" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>17</v>
@@ -903,11 +899,11 @@
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="15">
-        <v>46</v>
+      <c r="L8" s="3">
+        <v>0</v>
       </c>
-      <c r="M8" s="15">
-        <v>66.599999999999994</v>
+      <c r="M8" s="3">
+        <v>2000</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -925,13 +921,13 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>38</v>
@@ -939,11 +935,11 @@
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>15</v>
+      <c r="F9" s="3" t="s">
+        <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>60</v>
+      <c r="G9" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>17</v>
@@ -952,10 +948,10 @@
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
       <c r="L9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="3">
-        <v>2000</v>
+        <v>3</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -973,10 +969,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -988,10 +984,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>17</v>
@@ -1000,10 +996,10 @@
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
       <c r="L10" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M10" s="3">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1021,10 +1017,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1048,10 +1044,10 @@
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
       <c r="L11" s="3">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="M11" s="3">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1069,10 +1065,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -1095,11 +1091,11 @@
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="3">
-        <v>4</v>
+      <c r="L12" s="11">
+        <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1117,38 +1113,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>62</v>
+      <c r="B13" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="11">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
-        <v>160</v>
-      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1165,28 +1151,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>51</v>
+      <c r="B14" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="15"/>
+      <c r="L14" s="15">
+        <v>46</v>
+      </c>
+      <c r="M14" s="15">
+        <v>66.599999999999994</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -28988,16 +28984,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C64:C1007 C40:C52 C36:C38 C1:C33" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C64:C1007 C40:C52 C36:C38 C1:C7 C8:C33" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E40:E1007 E36:E38 E1:E33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E40:E1007 E36:E38 E1:E7 E8:E33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F40:F1007 F36:F38 F1:F33" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F40:F1007 F36:F38 F1:F7 F8:F33" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H40:H1007 H36:H38 H1:H33" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H40:H1007 H36:H38 H1:H7 H8:H33" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>